<commit_message>
lots of things after milion years
</commit_message>
<xml_diff>
--- a/Second semester/neural network/HW1/lbl0.xlsx
+++ b/Second semester/neural network/HW1/lbl0.xlsx
@@ -404,7 +404,7 @@
     </row>
     <row r="7" spans="1:1">
       <c r="A7">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="8" spans="1:1">
@@ -454,12 +454,12 @@
     </row>
     <row r="17" spans="1:1">
       <c r="A17">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="18" spans="1:1">
       <c r="A18">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="19" spans="1:1">
@@ -524,7 +524,7 @@
     </row>
     <row r="31" spans="1:1">
       <c r="A31">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="32" spans="1:1">
@@ -539,7 +539,7 @@
     </row>
     <row r="34" spans="1:1">
       <c r="A34">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="35" spans="1:1">
@@ -689,7 +689,7 @@
     </row>
     <row r="64" spans="1:1">
       <c r="A64">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="65" spans="1:1">
@@ -719,7 +719,7 @@
     </row>
     <row r="70" spans="1:1">
       <c r="A70">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="71" spans="1:1">
@@ -914,12 +914,12 @@
     </row>
     <row r="109" spans="1:1">
       <c r="A109">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="110" spans="1:1">
       <c r="A110">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="111" spans="1:1">
@@ -974,7 +974,7 @@
     </row>
     <row r="121" spans="1:1">
       <c r="A121">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="122" spans="1:1">
@@ -1069,7 +1069,7 @@
     </row>
     <row r="140" spans="1:1">
       <c r="A140">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="141" spans="1:1">
@@ -1114,7 +1114,7 @@
     </row>
     <row r="149" spans="1:1">
       <c r="A149">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="150" spans="1:1">
@@ -1129,7 +1129,7 @@
     </row>
     <row r="152" spans="1:1">
       <c r="A152">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="153" spans="1:1">
@@ -1189,7 +1189,7 @@
     </row>
     <row r="164" spans="1:1">
       <c r="A164">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="165" spans="1:1">
@@ -1234,22 +1234,22 @@
     </row>
     <row r="173" spans="1:1">
       <c r="A173">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="174" spans="1:1">
       <c r="A174">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="175" spans="1:1">
       <c r="A175">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="176" spans="1:1">
       <c r="A176">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="177" spans="1:1">
@@ -2584,7 +2584,7 @@
     </row>
     <row r="443" spans="1:1">
       <c r="A443">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="444" spans="1:1">
@@ -3644,7 +3644,7 @@
     </row>
     <row r="655" spans="1:1">
       <c r="A655">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="656" spans="1:1">
@@ -5089,7 +5089,7 @@
     </row>
     <row r="944" spans="1:1">
       <c r="A944">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="945" spans="1:1">
@@ -5239,7 +5239,7 @@
     </row>
     <row r="974" spans="1:1">
       <c r="A974">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="975" spans="1:1">
@@ -5599,7 +5599,7 @@
     </row>
     <row r="1046" spans="1:1">
       <c r="A1046">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="1047" spans="1:1">
@@ -5644,7 +5644,7 @@
     </row>
     <row r="1055" spans="1:1">
       <c r="A1055">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="1056" spans="1:1">
@@ -5789,7 +5789,7 @@
     </row>
     <row r="1084" spans="1:1">
       <c r="A1084">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="1085" spans="1:1">
@@ -6254,7 +6254,7 @@
     </row>
     <row r="1177" spans="1:1">
       <c r="A1177">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="1178" spans="1:1">
@@ -6379,7 +6379,7 @@
     </row>
     <row r="1202" spans="1:1">
       <c r="A1202">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="1203" spans="1:1">
@@ -6434,7 +6434,7 @@
     </row>
     <row r="1213" spans="1:1">
       <c r="A1213">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="1214" spans="1:1">
@@ -6444,7 +6444,7 @@
     </row>
     <row r="1215" spans="1:1">
       <c r="A1215">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="1216" spans="1:1">
@@ -6464,12 +6464,12 @@
     </row>
     <row r="1219" spans="1:1">
       <c r="A1219">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="1220" spans="1:1">
       <c r="A1220">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="1221" spans="1:1">

</xml_diff>